<commit_message>
interfaz req 3 - completed
</commit_message>
<xml_diff>
--- a/Datos/Requerimiento3/frecuencia_keywords_categorizadas.xlsx
+++ b/Datos/Requerimiento3/frecuencia_keywords_categorizadas.xlsx
@@ -483,7 +483,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Privacy</t>
+          <t>AI literacy</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -492,13 +492,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AI literacy</t>
+          <t>Transparency</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -513,7 +513,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Transparency</t>
+          <t>Privacy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">

</xml_diff>